<commit_message>
Updated S3. Sign-up and Login Test Cases.xlsx file
</commit_message>
<xml_diff>
--- a/Test Cases/S3. Sign-up and Login Test Cases.xlsx
+++ b/Test Cases/S3. Sign-up and Login Test Cases.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="225">
   <si>
     <t>Project Name</t>
   </si>
@@ -752,6 +752,12 @@
   </si>
   <si>
     <t>Login is not successful and user is notified that the password has changed</t>
+  </si>
+  <si>
+    <t>Pass</t>
+  </si>
+  <si>
+    <t>Password</t>
   </si>
 </sst>
 </file>
@@ -1859,13 +1865,13 @@
   </sheetPr>
   <dimension ref="A1:J97"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C99" sqref="C99"/>
+    <sheetView topLeftCell="A79" tabSelected="1" workbookViewId="0">
+      <selection activeCell="B100" sqref="B100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.63000000" defaultRowHeight="15.750000" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="6.43357120" customWidth="1" outlineLevel="0"/>
+    <col min="1" max="1" width="9.57642828" customWidth="1" outlineLevel="0"/>
     <col min="2" max="2" width="43.86214338" customWidth="1" outlineLevel="0"/>
     <col min="3" max="3" width="47.14785658" customWidth="1" outlineLevel="0"/>
     <col min="4" max="4" width="14.29071413" customWidth="1" outlineLevel="0"/>
@@ -3677,7 +3683,9 @@
       </c>
     </row>
     <row r="91" spans="1:10">
-      <c r="A91" s="15"/>
+      <c r="A91" s="15" t="s">
+        <v>224</v>
+      </c>
       <c r="B91" s="20" t="s">
         <v>163</v>
       </c>
@@ -3774,7 +3782,7 @@
   </sheetPr>
   <dimension ref="A1:F48"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A37" workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>

</xml_diff>